<commit_message>
Fixed all but 1 test by changing the peak annotation file paths in the study docs and a couple of code changes.
Details:

- I now expect a MzxmlNotColocatedWithAnnot error when the paths differ and there is no default fallback.
- I added an mzxml_filename argument to MSRunsLoader.get_msrun_sequence_from_dir for error reporting.

Files checked in: DataRepo/data/tests/same_name_mzxmls/mzxml_study_doc_same_seq.xlsx DataRepo/data/tests/small_obob/glucose/small_obob_animal_and_sample_table.xlsx DataRepo/loaders/msruns_loader.py DataRepo/tests/loaders/test_msruns_loader.py
</commit_message>
<xml_diff>
--- a/DataRepo/data/tests/same_name_mzxmls/mzxml_study_doc_same_seq.xlsx
+++ b/DataRepo/data/tests/same_name_mzxmls/mzxml_study_doc_same_seq.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rleach/PROJECT-LOCAL/TRACEBASE/tracebase/DataRepo/data/tests/same_name_mzxmls/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rleach/PROJECT-local/TRACEBASE/tracebase/DataRepo/data/tests/same_name_mzxmls/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AD1E172-DFB5-B748-B6E8-06DD16AAE26B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87E8387B-B30E-2A47-B29E-A5F840EA7B8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="680" yWindow="7040" windowWidth="29900" windowHeight="12800" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,12 +17,25 @@
     <sheet name="Peak Annotation Files" sheetId="11" r:id="rId2"/>
     <sheet name="Peak Annotation Details" sheetId="12" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="23">
   <si>
     <t>Sequence Name</t>
   </si>
@@ -82,12 +95,6 @@
   </si>
   <si>
     <t>accucor</t>
-  </si>
-  <si>
-    <t>DataRepo/data/tests/same_name_mzxmls/mzxmls/accucor1.xlsx</t>
-  </si>
-  <si>
-    <t>DataRepo/data/tests/same_name_mzxmls/mzxmls/accucor2.xlsx</t>
   </si>
   <si>
     <t>John Doe, polar-HILIC-25-min, QE, 1991-5-7</t>
@@ -418,7 +425,7 @@
     </row>
     <row r="2" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>14</v>
@@ -442,9 +449,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA025433-0E48-F741-90DE-D42669D25FD1}">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
@@ -456,10 +461,10 @@
   <sheetData>
     <row r="1" spans="1:3" ht="14" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>9</v>
@@ -467,24 +472,24 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>19</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>19</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -540,7 +545,7 @@
         <v>16</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="15" x14ac:dyDescent="0.2">
@@ -554,7 +559,7 @@
         <v>18</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>